<commit_message>
aeroscan agg ttest done
</commit_message>
<xml_diff>
--- a/obesity/ttresults.xlsx
+++ b/obesity/ttresults.xlsx
@@ -455,11 +455,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Statistic</t>
-        </is>
-      </c>
+      <c r="A1" s="1" t="inlineStr"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Effort level</t>
@@ -467,82 +463,82 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Respiratory rate (breaths/min)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Heart rate (beats/min)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Ventilation (l/min)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>O2 intake (l/min)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Relative O2 intake (ml/kg/min)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>CO2 expired (l/min)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Relative CO2 expired (ml/kg/min)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Respiratory exchange ratio</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Ventilation oxygen equivalent (l)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>O2 per pulse (l)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Fat energy (kcl/h)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Carbohydrates energy (kcal/h)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Fat energy %</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Carbohydrates energy %</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Carbohydrates energy (kcal/h)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Fat energy %</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Fat energy (kcl/h)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Heart rate (beats/min)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Total energy (kcal/h)</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Metabolic equivalent of task (MET) (3.5ml/kg/min)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>O2 intake (l/min)</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>O2 per pulse (l)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Relative CO2 expired (ml/kg/min)</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Relative O2 intake (ml/kg/min)</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Respiratory exchange ratio</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Respiratory rate (breaths/min)</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Total energy (kcal/h)</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Ventilation (l/min)</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Ventilation oxygen equivalent (l)</t>
         </is>
       </c>
     </row>
@@ -1054,52 +1050,52 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H11" t="n">
         <v>2.95</v>
       </c>
-      <c r="D11" t="n">
+      <c r="I11" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-2.84</v>
+      </c>
+      <c r="N11" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-2.54</v>
+      </c>
+      <c r="P11" t="n">
         <v>2.54</v>
       </c>
-      <c r="E11" t="n">
-        <v>3.23</v>
-      </c>
-      <c r="F11" t="n">
-        <v>-2.54</v>
-      </c>
-      <c r="G11" t="n">
-        <v>-2.84</v>
-      </c>
-      <c r="H11" t="n">
-        <v>3.29</v>
-      </c>
-      <c r="I11" t="n">
+      <c r="Q11" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="R11" t="n">
         <v>1.75</v>
-      </c>
-      <c r="J11" t="n">
-        <v>1.71</v>
-      </c>
-      <c r="K11" t="n">
-        <v>-0.12</v>
-      </c>
-      <c r="L11" t="n">
-        <v>2.95</v>
-      </c>
-      <c r="M11" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="N11" t="n">
-        <v>2.36</v>
-      </c>
-      <c r="O11" t="n">
-        <v>2.54</v>
-      </c>
-      <c r="P11" t="n">
-        <v>1.89</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>3.27</v>
-      </c>
-      <c r="R11" t="n">
-        <v>2.58</v>
       </c>
     </row>
     <row r="12">
@@ -1108,52 +1104,52 @@
         <v>2</v>
       </c>
       <c r="C12" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="H12" t="n">
         <v>2.5</v>
       </c>
-      <c r="D12" t="n">
+      <c r="I12" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="L12" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-0.57</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="O12" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="P12" t="n">
         <v>0.9</v>
       </c>
-      <c r="E12" t="n">
-        <v>1.51</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-0.9</v>
-      </c>
-      <c r="G12" t="n">
-        <v>-0.57</v>
-      </c>
-      <c r="H12" t="n">
-        <v>2.96</v>
-      </c>
-      <c r="I12" t="n">
+      <c r="Q12" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="R12" t="n">
         <v>1.61</v>
-      </c>
-      <c r="J12" t="n">
-        <v>1.56</v>
-      </c>
-      <c r="K12" t="n">
-        <v>-0.09</v>
-      </c>
-      <c r="L12" t="n">
-        <v>2.52</v>
-      </c>
-      <c r="M12" t="n">
-        <v>1.61</v>
-      </c>
-      <c r="N12" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="O12" t="n">
-        <v>2.99</v>
-      </c>
-      <c r="P12" t="n">
-        <v>1.57</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>2.95</v>
-      </c>
-      <c r="R12" t="n">
-        <v>2.66</v>
       </c>
     </row>
     <row r="13">
@@ -1162,52 +1158,52 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="H13" t="n">
         <v>2.91</v>
       </c>
-      <c r="D13" t="n">
+      <c r="I13" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-1.51</v>
+      </c>
+      <c r="N13" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="O13" t="n">
+        <v>-1.57</v>
+      </c>
+      <c r="P13" t="n">
         <v>0.72</v>
       </c>
-      <c r="E13" t="n">
-        <v>2.37</v>
-      </c>
-      <c r="F13" t="n">
-        <v>-1.57</v>
-      </c>
-      <c r="G13" t="n">
-        <v>-1.51</v>
-      </c>
-      <c r="H13" t="n">
-        <v>1.46</v>
-      </c>
-      <c r="I13" t="n">
+      <c r="Q13" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="R13" t="n">
         <v>2.06</v>
-      </c>
-      <c r="J13" t="n">
-        <v>2.12</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="L13" t="n">
-        <v>2.82</v>
-      </c>
-      <c r="M13" t="n">
-        <v>2.06</v>
-      </c>
-      <c r="N13" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="O13" t="n">
-        <v>1.91</v>
-      </c>
-      <c r="P13" t="n">
-        <v>2.16</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="R13" t="n">
-        <v>2.33</v>
       </c>
     </row>
     <row r="14">
@@ -1220,52 +1216,52 @@
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0054123155851389</v>
+        <v>0.015</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0154259247054392</v>
+        <v>0.002</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0025730371169</v>
+        <v>0.002</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0154259247051819</v>
+        <v>0.096</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0072898447994399</v>
+        <v>0.089</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0021639746230118</v>
+        <v>0.005</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0889740302585962</v>
+        <v>0.005</v>
       </c>
       <c r="J14" t="n">
-        <v>0.09550596651838381</v>
+        <v>0.023</v>
       </c>
       <c r="K14" t="n">
-        <v>0.9022859700969534</v>
+        <v>0.014</v>
       </c>
       <c r="L14" t="n">
-        <v>0.005446707903007</v>
+        <v>0.902</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0889740302722949</v>
+        <v>0.007</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0232460806166211</v>
+        <v>0.003</v>
       </c>
       <c r="O14" t="n">
-        <v>0.0151835286341653</v>
+        <v>0.015</v>
       </c>
       <c r="P14" t="n">
-        <v>0.06634275684172029</v>
+        <v>0.015</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.0022754287461671</v>
+        <v>0.066</v>
       </c>
       <c r="R14" t="n">
-        <v>0.013731411405932</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="15">
@@ -1274,52 +1270,52 @@
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>0.016900881923386</v>
+        <v>0.005</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3727481480122889</v>
+        <v>0.005</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1397839922130245</v>
+        <v>0.005</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3727481480113479</v>
+        <v>0.128</v>
       </c>
       <c r="G15" t="n">
-        <v>0.575050321029974</v>
+        <v>0.115</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0053295441976991</v>
+        <v>0.017</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1151313935539298</v>
+        <v>0.016</v>
       </c>
       <c r="J15" t="n">
-        <v>0.1281369842824651</v>
+        <v>0.021</v>
       </c>
       <c r="K15" t="n">
-        <v>0.9267550056012742</v>
+        <v>0.011</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0159375402442729</v>
+        <v>0.927</v>
       </c>
       <c r="M15" t="n">
-        <v>0.1151313935904721</v>
+        <v>0.575</v>
       </c>
       <c r="N15" t="n">
-        <v>0.0211927425378855</v>
+        <v>0.14</v>
       </c>
       <c r="O15" t="n">
-        <v>0.004870602912619</v>
+        <v>0.373</v>
       </c>
       <c r="P15" t="n">
-        <v>0.1245442912418619</v>
+        <v>0.373</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.0053493656249075</v>
+        <v>0.125</v>
       </c>
       <c r="R15" t="n">
-        <v>0.0113362155996073</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="16">
@@ -1328,52 +1324,52 @@
         <v>3</v>
       </c>
       <c r="C16" t="n">
-        <v>0.006036268441083</v>
+        <v>0.064</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4787904618116864</v>
+        <v>0.151</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0231421193107647</v>
+        <v>0.001</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1241783699635587</v>
+        <v>0.041</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1401675324489067</v>
+        <v>0.046</v>
       </c>
       <c r="H16" t="n">
-        <v>0.151240419035713</v>
+        <v>0.006</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0461784893530997</v>
+        <v>0.008</v>
       </c>
       <c r="J16" t="n">
-        <v>0.040514634569784</v>
+        <v>0.186</v>
       </c>
       <c r="K16" t="n">
-        <v>0.4282648264219885</v>
+        <v>0.025</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0075326510841564</v>
+        <v>0.428</v>
       </c>
       <c r="M16" t="n">
-        <v>0.046178489364613</v>
+        <v>0.14</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1858245234906667</v>
+        <v>0.023</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0640551143113037</v>
+        <v>0.124</v>
       </c>
       <c r="P16" t="n">
-        <v>0.0375356439129689</v>
+        <v>0.479</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.0011979865207242</v>
+        <v>0.038</v>
       </c>
       <c r="R16" t="n">
-        <v>0.025045201747917</v>
+        <v>0.046</v>
       </c>
     </row>
     <row r="17">
@@ -1386,52 +1382,52 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H17" t="n">
         <v>0.9</v>
       </c>
-      <c r="D17" t="n">
+      <c r="I17" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="M17" t="n">
+        <v>7.64</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="O17" t="n">
         <v>6.26</v>
       </c>
-      <c r="E17" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F17" t="n">
+      <c r="P17" t="n">
         <v>6.26</v>
       </c>
-      <c r="G17" t="n">
-        <v>7.64</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="I17" t="n">
+      <c r="Q17" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R17" t="n">
         <v>0.5600000000000001</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="L17" t="n">
-        <v>1.52</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>1.87</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="18">
@@ -1440,52 +1436,52 @@
         <v>2</v>
       </c>
       <c r="C18" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="H18" t="n">
         <v>1.66</v>
       </c>
-      <c r="D18" t="n">
+      <c r="I18" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="J18" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="K18" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O18" t="n">
         <v>0.74</v>
       </c>
-      <c r="E18" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="F18" t="n">
+      <c r="P18" t="n">
         <v>0.74</v>
       </c>
-      <c r="G18" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I18" t="n">
+      <c r="Q18" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="R18" t="n">
         <v>1.64</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="L18" t="n">
-        <v>3.82</v>
-      </c>
-      <c r="M18" t="n">
-        <v>1.64</v>
-      </c>
-      <c r="N18" t="n">
-        <v>4.26</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="R18" t="n">
-        <v>2.98</v>
       </c>
     </row>
     <row r="19">
@@ -1494,52 +1490,52 @@
         <v>3</v>
       </c>
       <c r="C19" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="H19" t="n">
         <v>1.88</v>
       </c>
-      <c r="D19" t="n">
+      <c r="I19" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="K19" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="M19" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2.84</v>
+      </c>
+      <c r="P19" t="n">
         <v>0.54</v>
       </c>
-      <c r="E19" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2.84</v>
-      </c>
-      <c r="G19" t="n">
-        <v>2.41</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="I19" t="n">
+      <c r="Q19" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="R19" t="n">
         <v>3.32</v>
-      </c>
-      <c r="J19" t="n">
-        <v>1.41</v>
-      </c>
-      <c r="K19" t="n">
-        <v>1.78</v>
-      </c>
-      <c r="L19" t="n">
-        <v>4.38</v>
-      </c>
-      <c r="M19" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="N19" t="n">
-        <v>2.44</v>
-      </c>
-      <c r="O19" t="n">
-        <v>1.38</v>
-      </c>
-      <c r="P19" t="n">
-        <v>1.49</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>4.11</v>
-      </c>
-      <c r="R19" t="n">
-        <v>2.82</v>
       </c>
     </row>
     <row r="20">
@@ -1552,52 +1548,52 @@
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>0.8960706095443677</v>
+        <v>0.487</v>
       </c>
       <c r="D20" t="n">
-        <v>6.258886586574272</v>
+        <v>0.755</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0738121886818444</v>
+        <v>0.176</v>
       </c>
       <c r="F20" t="n">
-        <v>6.258886586590324</v>
+        <v>0.886</v>
       </c>
       <c r="G20" t="n">
-        <v>7.635779531871387</v>
+        <v>0.457</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0978118156729685</v>
+        <v>0.347</v>
       </c>
       <c r="I20" t="n">
-        <v>0.5590051645320143</v>
+        <v>0.221</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0206475687153817</v>
+        <v>0.581</v>
       </c>
       <c r="K20" t="n">
-        <v>0.72263669645393</v>
+        <v>0.41</v>
       </c>
       <c r="L20" t="n">
-        <v>1.52232373798766</v>
+        <v>0.398</v>
       </c>
       <c r="M20" t="n">
-        <v>0.5590051643502699</v>
+        <v>0.007</v>
       </c>
       <c r="N20" t="n">
-        <v>0.3064372169664978</v>
+        <v>0.787</v>
       </c>
       <c r="O20" t="n">
-        <v>0.4889615357221444</v>
+        <v>0.015</v>
       </c>
       <c r="P20" t="n">
-        <v>0.0096841340961302</v>
+        <v>0.015</v>
       </c>
       <c r="Q20" t="n">
-        <v>1.867261614034268</v>
+        <v>0.922</v>
       </c>
       <c r="R20" t="n">
-        <v>0.6856187957464632</v>
+        <v>0.457</v>
       </c>
     </row>
     <row r="21">
@@ -1606,52 +1602,52 @@
         <v>2</v>
       </c>
       <c r="C21" t="n">
-        <v>1.664218492891498</v>
+        <v>0.741</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7438917346133158</v>
+        <v>0.699</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0503149387496927</v>
+        <v>0.093</v>
       </c>
       <c r="F21" t="n">
-        <v>0.743891734615845</v>
+        <v>0.629</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2735157805644108</v>
+        <v>0.205</v>
       </c>
       <c r="H21" t="n">
-        <v>0.1509430455790241</v>
+        <v>0.201</v>
       </c>
       <c r="I21" t="n">
-        <v>1.637153063703631</v>
+        <v>0.054</v>
       </c>
       <c r="J21" t="n">
-        <v>0.2350063700829613</v>
+        <v>0.043</v>
       </c>
       <c r="K21" t="n">
-        <v>0.6506609424845367</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="L21" t="n">
-        <v>3.823719050056603</v>
+        <v>0.422</v>
       </c>
       <c r="M21" t="n">
-        <v>1.637153063708898</v>
+        <v>0.603</v>
       </c>
       <c r="N21" t="n">
-        <v>4.256743471432856</v>
+        <v>0.823</v>
       </c>
       <c r="O21" t="n">
-        <v>0.1104096649472422</v>
+        <v>0.391</v>
       </c>
       <c r="P21" t="n">
-        <v>0.164361199048859</v>
+        <v>0.391</v>
       </c>
       <c r="Q21" t="n">
-        <v>2.895370311340646</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="R21" t="n">
-        <v>2.97836685255725</v>
+        <v>0.205</v>
       </c>
     </row>
     <row r="22">
@@ -1660,52 +1656,52 @@
         <v>3</v>
       </c>
       <c r="C22" t="n">
-        <v>1.880943552675588</v>
+        <v>0.243</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5365681717000976</v>
+        <v>0.502</v>
       </c>
       <c r="E22" t="n">
-        <v>0.5549005314833984</v>
+        <v>0.046</v>
       </c>
       <c r="F22" t="n">
-        <v>2.843439634743707</v>
+        <v>0.239</v>
       </c>
       <c r="G22" t="n">
-        <v>2.407527671786394</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="H22" t="n">
-        <v>0.4557628052951622</v>
+        <v>0.174</v>
       </c>
       <c r="I22" t="n">
-        <v>3.317996898080966</v>
+        <v>0.04</v>
       </c>
       <c r="J22" t="n">
-        <v>1.410284374695485</v>
+        <v>0.122</v>
       </c>
       <c r="K22" t="n">
-        <v>1.779561941278408</v>
+        <v>0.097</v>
       </c>
       <c r="L22" t="n">
-        <v>4.382549815911562</v>
+        <v>0.186</v>
       </c>
       <c r="M22" t="n">
-        <v>3.317996897910572</v>
+        <v>0.125</v>
       </c>
       <c r="N22" t="n">
-        <v>2.441852458137425</v>
+        <v>0.459</v>
       </c>
       <c r="O22" t="n">
-        <v>1.384885489169207</v>
+        <v>0.096</v>
       </c>
       <c r="P22" t="n">
-        <v>1.48752565532161</v>
+        <v>0.466</v>
       </c>
       <c r="Q22" t="n">
-        <v>4.111169245068285</v>
+        <v>0.226</v>
       </c>
       <c r="R22" t="n">
-        <v>2.815722153059042</v>
+        <v>0.07199999999999999</v>
       </c>
     </row>
     <row r="23">
@@ -1718,52 +1714,52 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>0.9</v>
+        <v>0.57</v>
       </c>
       <c r="D23" t="n">
-        <v>6.26</v>
+        <v>0.7</v>
       </c>
       <c r="E23" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.66</v>
       </c>
       <c r="F23" t="n">
-        <v>6.26</v>
+        <v>0.31</v>
       </c>
       <c r="G23" t="n">
-        <v>7.64</v>
+        <v>0.34</v>
       </c>
       <c r="H23" t="n">
-        <v>0.1</v>
+        <v>0.55</v>
       </c>
       <c r="I23" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="J23" t="n">
-        <v>0.02</v>
+        <v>0.61</v>
       </c>
       <c r="K23" t="n">
-        <v>0.72</v>
+        <v>0.68</v>
       </c>
       <c r="L23" t="n">
-        <v>1.52</v>
+        <v>-0.02</v>
       </c>
       <c r="M23" t="n">
-        <v>0.5600000000000001</v>
+        <v>-0.64</v>
       </c>
       <c r="N23" t="n">
-        <v>0.31</v>
+        <v>0.62</v>
       </c>
       <c r="O23" t="n">
-        <v>0.49</v>
+        <v>-0.59</v>
       </c>
       <c r="P23" t="n">
-        <v>0.01</v>
+        <v>0.59</v>
       </c>
       <c r="Q23" t="n">
-        <v>1.87</v>
+        <v>0.34</v>
       </c>
       <c r="R23" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="24">
@@ -1772,52 +1768,52 @@
         <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>1.66</v>
+        <v>0.63</v>
       </c>
       <c r="D24" t="n">
-        <v>0.74</v>
+        <v>0.64</v>
       </c>
       <c r="E24" t="n">
-        <v>0.05</v>
+        <v>0.62</v>
       </c>
       <c r="F24" t="n">
-        <v>0.74</v>
+        <v>0.32</v>
       </c>
       <c r="G24" t="n">
-        <v>0.27</v>
+        <v>0.35</v>
       </c>
       <c r="H24" t="n">
-        <v>0.15</v>
+        <v>0.53</v>
       </c>
       <c r="I24" t="n">
-        <v>1.64</v>
+        <v>0.57</v>
       </c>
       <c r="J24" t="n">
-        <v>0.24</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="K24" t="n">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
       <c r="L24" t="n">
-        <v>3.82</v>
+        <v>-0.02</v>
       </c>
       <c r="M24" t="n">
-        <v>1.64</v>
+        <v>-0.12</v>
       </c>
       <c r="N24" t="n">
-        <v>4.26</v>
+        <v>0.32</v>
       </c>
       <c r="O24" t="n">
-        <v>0.11</v>
+        <v>-0.2</v>
       </c>
       <c r="P24" t="n">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="Q24" t="n">
-        <v>2.9</v>
+        <v>0.32</v>
       </c>
       <c r="R24" t="n">
-        <v>2.98</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="25">
@@ -1826,52 +1822,52 @@
         <v>3</v>
       </c>
       <c r="C25" t="n">
-        <v>1.88</v>
+        <v>0.44</v>
       </c>
       <c r="D25" t="n">
-        <v>0.54</v>
+        <v>0.31</v>
       </c>
       <c r="E25" t="n">
-        <v>0.55</v>
+        <v>0.75</v>
       </c>
       <c r="F25" t="n">
-        <v>2.84</v>
+        <v>0.44</v>
       </c>
       <c r="G25" t="n">
-        <v>2.41</v>
+        <v>0.45</v>
       </c>
       <c r="H25" t="n">
-        <v>0.46</v>
+        <v>0.62</v>
       </c>
       <c r="I25" t="n">
-        <v>3.32</v>
+        <v>0.65</v>
       </c>
       <c r="J25" t="n">
-        <v>1.41</v>
+        <v>0.29</v>
       </c>
       <c r="K25" t="n">
-        <v>1.78</v>
+        <v>0.51</v>
       </c>
       <c r="L25" t="n">
-        <v>4.38</v>
+        <v>0.16</v>
       </c>
       <c r="M25" t="n">
-        <v>3.32</v>
+        <v>-0.35</v>
       </c>
       <c r="N25" t="n">
-        <v>2.44</v>
+        <v>0.53</v>
       </c>
       <c r="O25" t="n">
-        <v>1.38</v>
+        <v>-0.38</v>
       </c>
       <c r="P25" t="n">
-        <v>1.49</v>
+        <v>0.17</v>
       </c>
       <c r="Q25" t="n">
-        <v>4.11</v>
+        <v>0.45</v>
       </c>
       <c r="R25" t="n">
-        <v>2.82</v>
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>